<commit_message>
Auswertung Tag 4 fertig gemacht
</commit_message>
<xml_diff>
--- a/Tag 4 Auswertung/Enzymkinetik Auswertung.xlsx
+++ b/Tag 4 Auswertung/Enzymkinetik Auswertung.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maren\Documents\GitHub\Biochemie\Tag 4 Auswertung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\Documents\Uni\4. FS\Biochemie Praktikum\Biochemie\Tag 4 Auswertung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82228494-79F4-4F18-B065-3C617BB9BA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E24848-D0AF-4DA3-A88B-849709B8D06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="2" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="176">
   <si>
     <t>Application: Tecan i-control</t>
   </si>
@@ -640,13 +640,29 @@
   <si>
     <t>G6P</t>
   </si>
+  <si>
+    <t>Daten für Hanes-Woolf plot</t>
+  </si>
+  <si>
+    <t>vmax [mM/s]</t>
+  </si>
+  <si>
+    <t>Km [mM]</t>
+  </si>
+  <si>
+    <t>Ki[mM]</t>
+  </si>
+  <si>
+    <t>ATP [mM]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -780,7 +796,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -798,6 +814,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -807,9 +826,10 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -899,7 +919,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2281,7 +2301,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2319,7 +2339,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="672260095"/>
@@ -2399,7 +2419,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2437,7 +2457,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="672245951"/>
@@ -2479,7 +2499,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2516,7 +2536,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2597,7 +2617,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3979,7 +3999,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4017,7 +4037,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="672272575"/>
@@ -4101,7 +4121,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4139,7 +4159,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="672268831"/>
@@ -4181,7 +4201,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4218,7 +4238,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4299,7 +4319,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5681,7 +5701,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5719,7 +5739,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="877873759"/>
@@ -5804,7 +5824,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5842,7 +5862,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="877858783"/>
@@ -5884,7 +5904,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5921,7 +5941,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6002,7 +6022,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7592,7 +7612,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7630,7 +7650,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="672242207"/>
@@ -7710,7 +7730,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7748,7 +7768,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="672267999"/>
@@ -7790,7 +7810,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7827,7 +7847,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7918,7 +7938,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -9453,7 +9473,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9491,7 +9511,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="877851295"/>
@@ -9572,7 +9592,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9610,7 +9630,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="877854207"/>
@@ -9652,7 +9672,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9689,7 +9709,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9775,7 +9795,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -11157,7 +11177,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11195,7 +11215,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="49543583"/>
@@ -11277,7 +11297,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11315,7 +11335,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="49539423"/>
@@ -11357,7 +11377,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -11394,7 +11414,904 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Hanes-Woolf plot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet0!$F$187</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0mM ATP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.2510936132983378E-4"/>
+                  <c:y val="-1.2275048173784536E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet0!$E$189:$E$195</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet0!$F$189:$F$195</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3037.2625499405544</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3603.0316611191834</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4559.984431985923</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9616.7824832306433</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25445.105363860486</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39960.037017074465</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>52600.627637941056</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-733B-4A63-AC5D-112FF7D5E4B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet0!$G$187</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6mM ATP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.5305555555555555E-2"/>
+                  <c:y val="0.18719551171025853"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet0!$E$189:$E$195</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet0!$G$189:$G$195</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3271.1883031090306</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4839.2803556107383</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8972.9052172836618</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29026.858980105895</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70956.776453222221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>103435.12611472257</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>226208.52989621754</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-733B-4A63-AC5D-112FF7D5E4B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet0!$H$187</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>12mM ATP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.5611111111111115E-2"/>
+                  <c:y val="5.770658239047665E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet0!$E$189:$E$195</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet0!$H$189:$H$195</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6630.2220625001692</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13742.191858273463</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16188.047036681457</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32751.340428563675</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90401.931025695958</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>147151.92737394513</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>228803.20820112707</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-733B-4A63-AC5D-112FF7D5E4B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="213547392"/>
+        <c:axId val="213549056"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="213547392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>substrate concentration [mM]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="213549056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="213549056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>substrate conc./reaction</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> rate [s]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="213547392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="5"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11438,6 +12355,46 @@
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
   <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -14537,6 +15494,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -14750,6 +16223,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>146275</xdr:colOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>527275</xdr:colOff>
+      <xdr:row>225</xdr:row>
+      <xdr:rowOff>123143</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20A607F1-CB94-DB02-8EC9-3CE49E3EEF6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -15081,17 +16590,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L112" sqref="L112"/>
+    <sheetView tabSelected="1" topLeftCell="A182" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N204" sqref="N204"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="18" max="18" width="8.08984375" customWidth="1"/>
-    <col min="19" max="19" width="6.08984375" customWidth="1"/>
+    <col min="6" max="6" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.06640625" customWidth="1"/>
+    <col min="10" max="10" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.06640625" customWidth="1"/>
+    <col min="19" max="19" width="6.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15099,7 +16613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -15110,7 +16624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -15118,7 +16632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -15126,7 +16640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -15134,7 +16648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -15142,7 +16656,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -15150,7 +16664,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -15158,12 +16672,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -15179,7 +16693,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -15195,7 +16709,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -15211,17 +16725,17 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -15229,7 +16743,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -15237,7 +16751,7 @@
         <v>6.9444444444444447E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -15245,7 +16759,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -15256,7 +16770,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -15267,7 +16781,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -15275,7 +16789,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -15286,7 +16800,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -15294,7 +16808,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -15302,48 +16816,48 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="S32" s="14" t="s">
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="S32" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="T32" s="15"/>
-      <c r="U32" s="15"/>
-      <c r="V32" s="15"/>
-      <c r="W32" s="15"/>
-      <c r="X32" s="15"/>
-      <c r="Y32" s="15"/>
-      <c r="Z32" s="15"/>
-      <c r="AA32" s="15"/>
-      <c r="AB32" s="15"/>
-      <c r="AC32" s="15"/>
-      <c r="AD32" s="15"/>
-      <c r="AE32" s="15"/>
-      <c r="AF32" s="15"/>
-      <c r="AG32" s="15"/>
-      <c r="AH32" s="15"/>
+      <c r="T32" s="16"/>
+      <c r="U32" s="16"/>
+      <c r="V32" s="16"/>
+      <c r="W32" s="16"/>
+      <c r="X32" s="16"/>
+      <c r="Y32" s="16"/>
+      <c r="Z32" s="16"/>
+      <c r="AA32" s="16"/>
+      <c r="AB32" s="16"/>
+      <c r="AC32" s="16"/>
+      <c r="AD32" s="16"/>
+      <c r="AE32" s="16"/>
+      <c r="AF32" s="16"/>
+      <c r="AG32" s="16"/>
+      <c r="AH32" s="16"/>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="s">
         <v>37</v>
       </c>
@@ -15445,7 +16959,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A34" s="4" t="s">
         <v>38</v>
       </c>
@@ -15565,7 +17079,7 @@
         <v>4.6200007200241089E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="s">
         <v>39</v>
       </c>
@@ -15685,7 +17199,7 @@
         <v>3.540000319480896E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="s">
         <v>40</v>
       </c>
@@ -15805,7 +17319,7 @@
         <v>3.4800007939338684E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
         <v>41</v>
       </c>
@@ -15925,7 +17439,7 @@
         <v>0.14749999344348907</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="s">
         <v>42</v>
       </c>
@@ -16045,7 +17559,7 @@
         <v>0.13500000536441803</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A39" s="4" t="s">
         <v>43</v>
       </c>
@@ -16165,7 +17679,7 @@
         <v>0.14619998633861542</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A40" s="4" t="s">
         <v>44</v>
       </c>
@@ -16285,7 +17799,7 @@
         <v>0.1283000111579895</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
         <v>45</v>
       </c>
@@ -16405,7 +17919,7 @@
         <v>0.16079999506473541</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
         <v>46</v>
       </c>
@@ -16525,7 +18039,7 @@
         <v>0.12950000166893005</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="s">
         <v>47</v>
       </c>
@@ -16645,7 +18159,7 @@
         <v>0.49729996919631958</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
         <v>48</v>
       </c>
@@ -16765,7 +18279,7 @@
         <v>0.30149999260902405</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
         <v>49</v>
       </c>
@@ -16885,7 +18399,7 @@
         <v>0.3976999819278717</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A46" s="4" t="s">
         <v>50</v>
       </c>
@@ -17005,7 +18519,7 @@
         <v>0.32539999485015869</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A47" s="4" t="s">
         <v>51</v>
       </c>
@@ -17125,7 +18639,7 @@
         <v>0.46560001373291016</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="s">
         <v>52</v>
       </c>
@@ -17245,7 +18759,7 @@
         <v>0.62019997835159302</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A49" s="4" t="s">
         <v>53</v>
       </c>
@@ -17365,7 +18879,7 @@
         <v>0.32559996843338013</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A50" s="4" t="s">
         <v>54</v>
       </c>
@@ -17485,7 +18999,7 @@
         <v>0.26489996910095215</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A51" s="4" t="s">
         <v>55</v>
       </c>
@@ -17605,7 +19119,7 @@
         <v>0.23610001802444458</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A52" s="4" t="s">
         <v>56</v>
       </c>
@@ -17725,7 +19239,7 @@
         <v>0.46180003881454468</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A53" s="4" t="s">
         <v>57</v>
       </c>
@@ -17845,7 +19359,7 @@
         <v>0.81109997630119324</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A54" s="4" t="s">
         <v>58</v>
       </c>
@@ -17965,7 +19479,7 @@
         <v>0.66640001535415649</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A55" s="4" t="s">
         <v>59</v>
       </c>
@@ -18085,7 +19599,7 @@
         <v>0.51339997351169586</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A56" s="4" t="s">
         <v>60</v>
       </c>
@@ -18205,7 +19719,7 @@
         <v>0.49180002510547638</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A57" s="4" t="s">
         <v>61</v>
       </c>
@@ -18325,7 +19839,7 @@
         <v>0.64399999380111694</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A58" s="4" t="s">
         <v>62</v>
       </c>
@@ -18445,7 +19959,7 @@
         <v>0.26520001888275146</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A59" s="4" t="s">
         <v>63</v>
       </c>
@@ -18565,7 +20079,7 @@
         <v>0.20140001177787781</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A60" s="4" t="s">
         <v>64</v>
       </c>
@@ -18685,7 +20199,7 @@
         <v>0.31499998271465302</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A61" s="4" t="s">
         <v>65</v>
       </c>
@@ -18805,7 +20319,7 @@
         <v>0.8893999457359314</v>
       </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A62" s="4" t="s">
         <v>66</v>
       </c>
@@ -18925,7 +20439,7 @@
         <v>0.93120002746582031</v>
       </c>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A63" s="4" t="s">
         <v>67</v>
       </c>
@@ -19045,7 +20559,7 @@
         <v>1.0916000604629517</v>
       </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A64" s="4" t="s">
         <v>68</v>
       </c>
@@ -19165,7 +20679,7 @@
         <v>0.69689998030662537</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A65" s="4" t="s">
         <v>69</v>
       </c>
@@ -19285,7 +20799,7 @@
         <v>0.4966999888420105</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A66" s="4" t="s">
         <v>70</v>
       </c>
@@ -19405,7 +20919,7 @@
         <v>0.63359999656677246</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A67" s="4" t="s">
         <v>71</v>
       </c>
@@ -19525,7 +21039,7 @@
         <v>0.42549997568130493</v>
       </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A68" s="4" t="s">
         <v>72</v>
       </c>
@@ -19645,7 +21159,7 @@
         <v>0.37070000171661377</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A69" s="4" t="s">
         <v>73</v>
       </c>
@@ -19765,7 +21279,7 @@
         <v>0.3767000138759613</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A70" s="4" t="s">
         <v>74</v>
       </c>
@@ -19885,7 +21399,7 @@
         <v>0.60040000081062317</v>
       </c>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A71" s="4" t="s">
         <v>75</v>
       </c>
@@ -20005,7 +21519,7 @@
         <v>0.94280004501342773</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A72" s="4" t="s">
         <v>76</v>
       </c>
@@ -20125,7 +21639,7 @@
         <v>1.2834999859333038</v>
       </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A73" s="4" t="s">
         <v>77</v>
       </c>
@@ -20245,7 +21759,7 @@
         <v>0.40209999680519104</v>
       </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A74" s="4" t="s">
         <v>78</v>
       </c>
@@ -20365,7 +21879,7 @@
         <v>0.48459997773170471</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A75" s="4" t="s">
         <v>79</v>
       </c>
@@ -20485,7 +21999,7 @@
         <v>0.46299999952316284</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A76" s="4" t="s">
         <v>80</v>
       </c>
@@ -20605,7 +22119,7 @@
         <v>0.40410000085830688</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A77" s="4" t="s">
         <v>81</v>
       </c>
@@ -20725,7 +22239,7 @@
         <v>0.40390001237392426</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A78" s="4" t="s">
         <v>82</v>
       </c>
@@ -20845,7 +22359,7 @@
         <v>0.38969996571540833</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A79" s="4" t="s">
         <v>83</v>
       </c>
@@ -20965,7 +22479,7 @@
         <v>0.84519997239112854</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A80" s="4" t="s">
         <v>84</v>
       </c>
@@ -21085,7 +22599,7 @@
         <v>0.84869995713233948</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A81" s="4" t="s">
         <v>85</v>
       </c>
@@ -21205,7 +22719,7 @@
         <v>1.0161999762058258</v>
       </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A82" s="4" t="s">
         <v>86</v>
       </c>
@@ -21325,7 +22839,7 @@
         <v>0.59079998731613159</v>
       </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A83" s="4" t="s">
         <v>87</v>
       </c>
@@ -21445,7 +22959,7 @@
         <v>0.37459999322891235</v>
       </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A84" s="4" t="s">
         <v>88</v>
       </c>
@@ -21565,7 +23079,7 @@
         <v>0.40329998731613159</v>
       </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A85" s="4" t="s">
         <v>89</v>
       </c>
@@ -21685,7 +23199,7 @@
         <v>0.24699999392032623</v>
       </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A86" s="4" t="s">
         <v>90</v>
       </c>
@@ -21805,7 +23319,7 @@
         <v>0.53339999914169312</v>
       </c>
     </row>
-    <row r="87" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A87" s="4" t="s">
         <v>91</v>
       </c>
@@ -21925,7 +23439,7 @@
         <v>0.36090001463890076</v>
       </c>
     </row>
-    <row r="88" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A88" s="4" t="s">
         <v>92</v>
       </c>
@@ -22045,7 +23559,7 @@
         <v>0.76409995555877686</v>
       </c>
     </row>
-    <row r="89" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A89" s="4" t="s">
         <v>93</v>
       </c>
@@ -22165,7 +23679,7 @@
         <v>0.91800004243850708</v>
       </c>
     </row>
-    <row r="90" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A90" s="4" t="s">
         <v>94</v>
       </c>
@@ -22285,7 +23799,7 @@
         <v>0.74010005593299866</v>
       </c>
     </row>
-    <row r="91" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A91" s="4" t="s">
         <v>95</v>
       </c>
@@ -22405,7 +23919,7 @@
         <v>0.40960001945495605</v>
       </c>
     </row>
-    <row r="92" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A92" s="4" t="s">
         <v>96</v>
       </c>
@@ -22525,7 +24039,7 @@
         <v>0.4506000280380249</v>
       </c>
     </row>
-    <row r="93" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A93" s="4" t="s">
         <v>97</v>
       </c>
@@ -22645,7 +24159,7 @@
         <v>0.45669999718666077</v>
       </c>
     </row>
-    <row r="94" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A94" s="4" t="s">
         <v>98</v>
       </c>
@@ -22765,7 +24279,7 @@
         <v>0.30530001223087311</v>
       </c>
     </row>
-    <row r="95" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A95" s="4" t="s">
         <v>99</v>
       </c>
@@ -22885,7 +24399,7 @@
         <v>0.35990001261234283</v>
       </c>
     </row>
-    <row r="96" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A96" s="4" t="s">
         <v>100</v>
       </c>
@@ -23005,7 +24519,7 @@
         <v>0.32759998738765717</v>
       </c>
     </row>
-    <row r="97" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A97" s="4" t="s">
         <v>101</v>
       </c>
@@ -23125,7 +24639,7 @@
         <v>1.0455000400543213</v>
       </c>
     </row>
-    <row r="98" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A98" s="4" t="s">
         <v>102</v>
       </c>
@@ -23245,7 +24759,7 @@
         <v>0.815900057554245</v>
       </c>
     </row>
-    <row r="99" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A99" s="4" t="s">
         <v>103</v>
       </c>
@@ -23365,7 +24879,7 @@
         <v>0.75529998540878296</v>
       </c>
     </row>
-    <row r="100" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A100" s="4" t="s">
         <v>104</v>
       </c>
@@ -23485,7 +24999,7 @@
         <v>0.36609998345375061</v>
       </c>
     </row>
-    <row r="101" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A101" s="4" t="s">
         <v>105</v>
       </c>
@@ -23605,7 +25119,7 @@
         <v>0.33949999511241913</v>
       </c>
     </row>
-    <row r="102" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A102" s="4" t="s">
         <v>106</v>
       </c>
@@ -23725,7 +25239,7 @@
         <v>0.33190000057220459</v>
       </c>
     </row>
-    <row r="103" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A103" s="4" t="s">
         <v>107</v>
       </c>
@@ -23845,7 +25359,7 @@
         <v>0.2988000214099884</v>
       </c>
     </row>
-    <row r="104" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A104" s="4" t="s">
         <v>108</v>
       </c>
@@ -23965,7 +25479,7 @@
         <v>0.37960003316402435</v>
       </c>
     </row>
-    <row r="105" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A105" s="4" t="s">
         <v>109</v>
       </c>
@@ -24085,45 +25599,45 @@
         <v>0.2718999981880188</v>
       </c>
     </row>
-    <row r="107" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B107" s="16" t="s">
+    <row r="107" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B107" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C107" s="16"/>
-      <c r="D107" s="16"/>
-      <c r="E107" s="16"/>
-      <c r="F107" s="16"/>
-      <c r="G107" s="16"/>
-      <c r="H107" s="16"/>
-      <c r="I107" s="16"/>
-      <c r="J107" s="16"/>
-      <c r="K107" s="16"/>
-      <c r="L107" s="16"/>
-      <c r="M107" s="16"/>
-      <c r="N107" s="16"/>
-      <c r="O107" s="16"/>
-      <c r="P107" s="16"/>
-      <c r="Q107" s="16"/>
-      <c r="R107" s="16" t="s">
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="13"/>
+      <c r="G107" s="13"/>
+      <c r="H107" s="13"/>
+      <c r="I107" s="13"/>
+      <c r="J107" s="13"/>
+      <c r="K107" s="13"/>
+      <c r="L107" s="13"/>
+      <c r="M107" s="13"/>
+      <c r="N107" s="13"/>
+      <c r="O107" s="13"/>
+      <c r="P107" s="13"/>
+      <c r="Q107" s="13"/>
+      <c r="R107" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="S107" s="16"/>
-      <c r="T107" s="16"/>
-      <c r="U107" s="16"/>
-      <c r="V107" s="16"/>
-      <c r="W107" s="16"/>
-      <c r="X107" s="16"/>
-      <c r="Y107" s="16"/>
-      <c r="Z107" s="16"/>
-      <c r="AA107" s="16"/>
-      <c r="AB107" s="16"/>
-      <c r="AC107" s="16"/>
-      <c r="AD107" s="16"/>
-      <c r="AE107" s="16"/>
-      <c r="AF107" s="16"/>
-      <c r="AG107" s="16"/>
+      <c r="S107" s="13"/>
+      <c r="T107" s="13"/>
+      <c r="U107" s="13"/>
+      <c r="V107" s="13"/>
+      <c r="W107" s="13"/>
+      <c r="X107" s="13"/>
+      <c r="Y107" s="13"/>
+      <c r="Z107" s="13"/>
+      <c r="AA107" s="13"/>
+      <c r="AB107" s="13"/>
+      <c r="AC107" s="13"/>
+      <c r="AD107" s="13"/>
+      <c r="AE107" s="13"/>
+      <c r="AF107" s="13"/>
+      <c r="AG107" s="13"/>
     </row>
-    <row r="108" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B108" s="5">
         <v>0</v>
       </c>
@@ -24221,7 +25735,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="109" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A109" s="4" t="s">
         <v>112</v>
       </c>
@@ -24354,7 +25868,7 @@
         <v>6.4156068038873394E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A110" s="4" t="s">
         <v>113</v>
       </c>
@@ -24487,7 +26001,7 @@
         <v>6.8724000450112489E-3</v>
       </c>
     </row>
-    <row r="111" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A111" s="4" t="s">
         <v>114</v>
       </c>
@@ -24620,7 +26134,7 @@
         <v>1.8427237619633167E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A112" s="4" t="s">
         <v>115</v>
       </c>
@@ -24753,7 +26267,7 @@
         <v>9.7904908151061662E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A113" s="4" t="s">
         <v>116</v>
       </c>
@@ -24886,7 +26400,7 @@
         <v>0.14745859567308361</v>
       </c>
     </row>
-    <row r="114" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A114" s="4" t="s">
         <v>117</v>
       </c>
@@ -25019,7 +26533,7 @@
         <v>4.5687650089435018E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A115" s="4" t="s">
         <v>118</v>
       </c>
@@ -25152,7 +26666,7 @@
         <v>0.17550388192585203</v>
       </c>
     </row>
-    <row r="116" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A116" s="4" t="s">
         <v>119</v>
       </c>
@@ -25285,7 +26799,7 @@
         <v>8.234860203397748E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A117" s="4" t="s">
         <v>120</v>
       </c>
@@ -25418,7 +26932,7 @@
         <v>5.6943584217300509E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A118" s="4" t="s">
         <v>121</v>
       </c>
@@ -25551,7 +27065,7 @@
         <v>0.10673979561978933</v>
       </c>
     </row>
-    <row r="119" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A119" s="4" t="s">
         <v>122</v>
       </c>
@@ -25684,7 +27198,7 @@
         <v>0.10232997006330193</v>
       </c>
     </row>
-    <row r="120" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A120" s="4" t="s">
         <v>123</v>
       </c>
@@ -25817,7 +27331,7 @@
         <v>3.0056817209650748E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A121" s="4" t="s">
         <v>124</v>
       </c>
@@ -25950,7 +27464,7 @@
         <v>0.34155034516341698</v>
       </c>
     </row>
-    <row r="122" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A122" s="4" t="s">
         <v>125</v>
       </c>
@@ -26083,7 +27597,7 @@
         <v>4.2781647627874224E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A123" s="4" t="s">
         <v>126</v>
       </c>
@@ -26216,7 +27730,7 @@
         <v>8.2567379819416635E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A124" s="4" t="s">
         <v>127</v>
       </c>
@@ -26349,7 +27863,7 @@
         <v>9.7732208600366646E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A125" s="4" t="s">
         <v>128</v>
       </c>
@@ -26482,7 +27996,7 @@
         <v>0.11741832416898711</v>
       </c>
     </row>
-    <row r="126" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A126" s="4" t="s">
         <v>129</v>
       </c>
@@ -26615,7 +28129,7 @@
         <v>0.14419571327652467</v>
       </c>
     </row>
-    <row r="127" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A127" s="4" t="s">
         <v>130</v>
       </c>
@@ -26748,7 +28262,7 @@
         <v>9.6531201451737894E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A128" s="4" t="s">
         <v>131</v>
       </c>
@@ -26881,7 +28395,7 @@
         <v>2.5614508355464968E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A129" s="4" t="s">
         <v>132</v>
       </c>
@@ -27014,7 +28528,7 @@
         <v>2.7452202592764183E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A130" s="4" t="s">
         <v>133</v>
       </c>
@@ -27147,7 +28661,7 @@
         <v>0.1530820000437369</v>
       </c>
     </row>
-    <row r="131" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A131" s="4" t="s">
         <v>134</v>
       </c>
@@ -27280,7 +28794,7 @@
         <v>1.7958090682977698E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A132" s="4" t="s">
         <v>135</v>
       </c>
@@ -27413,45 +28927,45 @@
         <v>5.6052877836657841E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="B134" s="16" t="s">
+    <row r="134" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="B134" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="C134" s="16"/>
-      <c r="D134" s="16"/>
-      <c r="E134" s="16"/>
-      <c r="F134" s="16"/>
-      <c r="G134" s="16"/>
-      <c r="H134" s="16"/>
-      <c r="I134" s="16"/>
-      <c r="J134" s="16"/>
-      <c r="K134" s="16"/>
-      <c r="L134" s="16"/>
-      <c r="M134" s="16"/>
-      <c r="N134" s="16"/>
-      <c r="O134" s="16"/>
-      <c r="P134" s="16"/>
-      <c r="Q134" s="16"/>
-      <c r="R134" s="16" t="s">
+      <c r="C134" s="13"/>
+      <c r="D134" s="13"/>
+      <c r="E134" s="13"/>
+      <c r="F134" s="13"/>
+      <c r="G134" s="13"/>
+      <c r="H134" s="13"/>
+      <c r="I134" s="13"/>
+      <c r="J134" s="13"/>
+      <c r="K134" s="13"/>
+      <c r="L134" s="13"/>
+      <c r="M134" s="13"/>
+      <c r="N134" s="13"/>
+      <c r="O134" s="13"/>
+      <c r="P134" s="13"/>
+      <c r="Q134" s="13"/>
+      <c r="R134" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="S134" s="16"/>
-      <c r="T134" s="16"/>
-      <c r="U134" s="16"/>
-      <c r="V134" s="16"/>
-      <c r="W134" s="16"/>
-      <c r="X134" s="16"/>
-      <c r="Y134" s="16"/>
-      <c r="Z134" s="16"/>
-      <c r="AA134" s="16"/>
-      <c r="AB134" s="16"/>
-      <c r="AC134" s="16"/>
-      <c r="AD134" s="16"/>
-      <c r="AE134" s="16"/>
-      <c r="AF134" s="16"/>
-      <c r="AG134" s="16"/>
+      <c r="S134" s="13"/>
+      <c r="T134" s="13"/>
+      <c r="U134" s="13"/>
+      <c r="V134" s="13"/>
+      <c r="W134" s="13"/>
+      <c r="X134" s="13"/>
+      <c r="Y134" s="13"/>
+      <c r="Z134" s="13"/>
+      <c r="AA134" s="13"/>
+      <c r="AB134" s="13"/>
+      <c r="AC134" s="13"/>
+      <c r="AD134" s="13"/>
+      <c r="AE134" s="13"/>
+      <c r="AF134" s="13"/>
+      <c r="AG134" s="13"/>
     </row>
-    <row r="135" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:33" x14ac:dyDescent="0.45">
       <c r="B135" s="5">
         <v>0</v>
       </c>
@@ -27549,7 +29063,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="136" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A136" s="4" t="s">
         <v>112</v>
       </c>
@@ -27682,7 +29196,7 @@
         <v>6.4156068038873394E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A137" s="4" t="s">
         <v>113</v>
       </c>
@@ -27815,7 +29329,7 @@
         <v>9.7190413497083763E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A138" s="4" t="s">
         <v>114</v>
       </c>
@@ -27948,7 +29462,7 @@
         <v>2.6060049358756932E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A139" s="4" t="s">
         <v>115</v>
       </c>
@@ -28081,7 +29595,7 @@
         <v>9.8114886998507553E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A140" s="4" t="s">
         <v>116</v>
       </c>
@@ -28214,7 +29728,7 @@
         <v>0.14761865505503233</v>
       </c>
     </row>
-    <row r="141" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A141" s="4" t="s">
         <v>117</v>
       </c>
@@ -28347,7 +29861,7 @@
         <v>4.9263825034045777E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A142" s="4" t="s">
         <v>118</v>
       </c>
@@ -28480,7 +29994,7 @@
         <v>0.17562110517163221</v>
       </c>
     </row>
-    <row r="143" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A143" s="4" t="s">
         <v>119</v>
       </c>
@@ -28613,7 +30127,7 @@
         <v>8.2634872416728941E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A144" s="4" t="s">
         <v>120</v>
       </c>
@@ -28746,7 +30260,7 @@
         <v>5.9850938754569413E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A145" s="4" t="s">
         <v>121</v>
       </c>
@@ -28879,7 +30393,7 @@
         <v>0.10693242716602146</v>
       </c>
     </row>
-    <row r="146" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A146" s="4" t="s">
         <v>122</v>
       </c>
@@ -29012,7 +30526,7 @@
         <v>0.10256048291391251</v>
       </c>
     </row>
-    <row r="147" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A147" s="4" t="s">
         <v>123</v>
       </c>
@@ -29145,7 +30659,7 @@
         <v>3.5255855500395693E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A148" s="4" t="s">
         <v>124</v>
       </c>
@@ -29278,7 +30792,7 @@
         <v>0.34161059452527431</v>
       </c>
     </row>
-    <row r="149" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A149" s="4" t="s">
         <v>125</v>
       </c>
@@ -29411,7 +30925,7 @@
         <v>4.3330119502884672E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A150" s="4" t="s">
         <v>126</v>
       </c>
@@ -29544,7 +31058,7 @@
         <v>2.0192493862642671E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A151" s="4" t="s">
         <v>127</v>
       </c>
@@ -29677,7 +31191,7 @@
         <v>9.7942557698722912E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A152" s="4" t="s">
         <v>128</v>
       </c>
@@ -29810,7 +31324,7 @@
         <v>0.11761927024527917</v>
       </c>
     </row>
-    <row r="153" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A153" s="4" t="s">
         <v>129</v>
       </c>
@@ -29943,7 +31457,7 @@
         <v>0.14536838312926278</v>
       </c>
     </row>
-    <row r="154" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A154" s="4" t="s">
         <v>130</v>
       </c>
@@ -30076,7 +31590,7 @@
         <v>9.6744161913668414E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A155" s="4" t="s">
         <v>131</v>
       </c>
@@ -30209,7 +31723,7 @@
         <v>2.6520424594467851E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A156" s="4" t="s">
         <v>132</v>
       </c>
@@ -30342,7 +31856,7 @@
         <v>3.3063371175435098E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A157" s="4" t="s">
         <v>133</v>
       </c>
@@ -30475,7 +31989,7 @@
         <v>0.15321637885047651</v>
       </c>
     </row>
-    <row r="158" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A158" s="4" t="s">
         <v>134</v>
       </c>
@@ -30608,7 +32122,7 @@
         <v>1.9228179928342699E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A159" s="4" t="s">
         <v>135</v>
       </c>
@@ -30741,45 +32255,45 @@
         <v>5.9004137143608089E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="B160" s="16" t="s">
+    <row r="160" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="B160" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="C160" s="16"/>
-      <c r="D160" s="16"/>
-      <c r="E160" s="16"/>
-      <c r="F160" s="16"/>
-      <c r="G160" s="16"/>
-      <c r="H160" s="16"/>
-      <c r="I160" s="16"/>
-      <c r="J160" s="16"/>
-      <c r="K160" s="16"/>
-      <c r="L160" s="16"/>
-      <c r="M160" s="16"/>
-      <c r="N160" s="16"/>
-      <c r="O160" s="16"/>
-      <c r="P160" s="16"/>
-      <c r="Q160" s="16"/>
-      <c r="R160" s="16" t="s">
+      <c r="C160" s="13"/>
+      <c r="D160" s="13"/>
+      <c r="E160" s="13"/>
+      <c r="F160" s="13"/>
+      <c r="G160" s="13"/>
+      <c r="H160" s="13"/>
+      <c r="I160" s="13"/>
+      <c r="J160" s="13"/>
+      <c r="K160" s="13"/>
+      <c r="L160" s="13"/>
+      <c r="M160" s="13"/>
+      <c r="N160" s="13"/>
+      <c r="O160" s="13"/>
+      <c r="P160" s="13"/>
+      <c r="Q160" s="13"/>
+      <c r="R160" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="S160" s="16"/>
-      <c r="T160" s="16"/>
-      <c r="U160" s="16"/>
-      <c r="V160" s="16"/>
-      <c r="W160" s="16"/>
-      <c r="X160" s="16"/>
-      <c r="Y160" s="16"/>
-      <c r="Z160" s="16"/>
-      <c r="AA160" s="16"/>
-      <c r="AB160" s="16"/>
-      <c r="AC160" s="16"/>
-      <c r="AD160" s="16"/>
-      <c r="AE160" s="16"/>
-      <c r="AF160" s="16"/>
-      <c r="AG160" s="16"/>
+      <c r="S160" s="13"/>
+      <c r="T160" s="13"/>
+      <c r="U160" s="13"/>
+      <c r="V160" s="13"/>
+      <c r="W160" s="13"/>
+      <c r="X160" s="13"/>
+      <c r="Y160" s="13"/>
+      <c r="Z160" s="13"/>
+      <c r="AA160" s="13"/>
+      <c r="AB160" s="13"/>
+      <c r="AC160" s="13"/>
+      <c r="AD160" s="13"/>
+      <c r="AE160" s="13"/>
+      <c r="AF160" s="13"/>
+      <c r="AG160" s="13"/>
     </row>
-    <row r="161" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:33" x14ac:dyDescent="0.45">
       <c r="B161" s="5">
         <v>0</v>
       </c>
@@ -30877,7 +32391,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="162" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A162" s="4" t="s">
         <v>140</v>
       </c>
@@ -31010,7 +32524,7 @@
         <v>1.3223692810386963E-3</v>
       </c>
     </row>
-    <row r="163" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A163" s="4" t="s">
         <v>141</v>
       </c>
@@ -31143,7 +32657,7 @@
         <v>2.0032651804988821E-3</v>
       </c>
     </row>
-    <row r="164" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A164" s="4" t="s">
         <v>142</v>
       </c>
@@ -31276,7 +32790,7 @@
         <v>5.3714340338768514E-3</v>
       </c>
     </row>
-    <row r="165" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A165" s="4" t="s">
         <v>143</v>
       </c>
@@ -31409,7 +32923,7 @@
         <v>2.0223202036133966E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A166" s="4" t="s">
         <v>144</v>
       </c>
@@ -31542,7 +33056,7 @@
         <v>3.0426798387136678E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A167" s="4" t="s">
         <v>145</v>
       </c>
@@ -31675,7 +33189,7 @@
         <v>1.0154139878400069E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A168" s="4" t="s">
         <v>146</v>
       </c>
@@ -31808,7 +33322,7 @@
         <v>3.6198595344140529E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A169" s="4" t="s">
         <v>147</v>
       </c>
@@ -31941,7 +33455,7 @@
         <v>1.7032499055307307E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A170" s="4" t="s">
         <v>149</v>
       </c>
@@ -32074,7 +33588,7 @@
         <v>1.233633002608818E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A171" s="4" t="s">
         <v>150</v>
       </c>
@@ -32207,7 +33721,7 @@
         <v>2.2040651984092146E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A172" s="4" t="s">
         <v>151</v>
       </c>
@@ -32340,7 +33854,7 @@
         <v>2.1139517461025745E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A173" s="4" t="s">
         <v>152</v>
       </c>
@@ -32473,7 +33987,7 @@
         <v>7.2668512450316785E-3</v>
       </c>
     </row>
-    <row r="174" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A174" s="4" t="s">
         <v>153</v>
       </c>
@@ -32606,7 +34120,7 @@
         <v>7.0411945445888843E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A175" s="4" t="s">
         <v>154</v>
       </c>
@@ -32739,7 +34253,7 @@
         <v>8.9310989164161653E-3</v>
       </c>
     </row>
-    <row r="176" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A176" s="4" t="s">
         <v>155</v>
       </c>
@@ -32872,7 +34386,7 @@
         <v>4.162027756336604E-3</v>
       </c>
     </row>
-    <row r="177" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A177" s="4" t="s">
         <v>156</v>
       </c>
@@ -33005,7 +34519,7 @@
         <v>2.0187681939715332E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A178" s="4" t="s">
         <v>157</v>
       </c>
@@ -33138,7 +34652,7 @@
         <v>2.4243398104806489E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A179" s="4" t="s">
         <v>158</v>
       </c>
@@ -33271,7 +34785,7 @@
         <v>2.996297780716934E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A180" s="4" t="s">
         <v>159</v>
       </c>
@@ -33404,7 +34918,7 @@
         <v>1.9940671513246848E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A181" s="4" t="s">
         <v>160</v>
       </c>
@@ -33537,7 +35051,7 @@
         <v>5.4663254585019068E-3</v>
       </c>
     </row>
-    <row r="182" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A182" s="4" t="s">
         <v>161</v>
       </c>
@@ -33670,7 +35184,7 @@
         <v>6.8149417048880981E-3</v>
       </c>
     </row>
-    <row r="183" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A183" s="4" t="s">
         <v>162</v>
       </c>
@@ -33803,7 +35317,7 @@
         <v>3.1580587610371115E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A184" s="4" t="s">
         <v>163</v>
       </c>
@@ -33936,7 +35450,7 @@
         <v>3.9632657120007211E-3</v>
       </c>
     </row>
-    <row r="185" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A185" s="4" t="s">
         <v>164</v>
       </c>
@@ -34069,44 +35583,48 @@
         <v>1.2161789336220646E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A186" s="16" t="s">
+    <row r="186" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A186" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="B186" s="16"/>
-      <c r="C186" s="16"/>
-      <c r="D186" s="16"/>
-      <c r="E186" s="16"/>
-      <c r="F186" s="16"/>
-      <c r="G186" s="16"/>
-      <c r="H186" s="8"/>
+      <c r="B186" s="13"/>
+      <c r="C186" s="13"/>
+      <c r="D186" s="13"/>
+      <c r="E186" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="F186" s="13"/>
+      <c r="G186" s="13"/>
+      <c r="H186" s="13"/>
       <c r="I186" s="8"/>
       <c r="J186" s="8"/>
       <c r="K186" s="8"/>
       <c r="L186" s="8"/>
       <c r="M186" s="8"/>
-      <c r="N186" s="8"/>
-      <c r="O186" s="8"/>
-      <c r="P186" s="8"/>
+      <c r="N186" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="O186" s="13"/>
+      <c r="P186" s="13"/>
       <c r="Q186" s="8"/>
-      <c r="R186" s="16"/>
-      <c r="S186" s="16"/>
-      <c r="T186" s="16"/>
-      <c r="U186" s="16"/>
-      <c r="V186" s="16"/>
-      <c r="W186" s="16"/>
-      <c r="X186" s="16"/>
-      <c r="Y186" s="16"/>
-      <c r="Z186" s="16"/>
-      <c r="AA186" s="16"/>
-      <c r="AB186" s="16"/>
-      <c r="AC186" s="16"/>
-      <c r="AD186" s="16"/>
-      <c r="AE186" s="16"/>
-      <c r="AF186" s="16"/>
-      <c r="AG186" s="16"/>
+      <c r="R186" s="13"/>
+      <c r="S186" s="13"/>
+      <c r="T186" s="13"/>
+      <c r="U186" s="13"/>
+      <c r="V186" s="13"/>
+      <c r="W186" s="13"/>
+      <c r="X186" s="13"/>
+      <c r="Y186" s="13"/>
+      <c r="Z186" s="13"/>
+      <c r="AA186" s="13"/>
+      <c r="AB186" s="13"/>
+      <c r="AC186" s="13"/>
+      <c r="AD186" s="13"/>
+      <c r="AE186" s="13"/>
+      <c r="AF186" s="13"/>
+      <c r="AG186" s="13"/>
     </row>
-    <row r="187" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A187" s="12" t="s">
         <v>170</v>
       </c>
@@ -34119,18 +35637,43 @@
       <c r="D187" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="E187" s="5"/>
-      <c r="F187" s="5"/>
-      <c r="G187" s="5"/>
+      <c r="E187" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="F187" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="G187" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="H187" s="5" t="s">
+        <v>169</v>
+      </c>
       <c r="I187" s="5"/>
-      <c r="J187" s="5"/>
-      <c r="K187" s="5"/>
-      <c r="L187" s="5"/>
-      <c r="M187" s="5"/>
-      <c r="N187" s="5"/>
-      <c r="O187" s="5"/>
-      <c r="P187" s="5"/>
-      <c r="Q187" s="5"/>
+      <c r="J187" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="K187" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="L187" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="M187" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="N187" s="5">
+        <v>0</v>
+      </c>
+      <c r="O187" s="5">
+        <v>6</v>
+      </c>
+      <c r="P187" s="5">
+        <v>12</v>
+      </c>
+      <c r="Q187" s="5" t="s">
+        <v>175</v>
+      </c>
       <c r="R187" s="5"/>
       <c r="S187" s="5"/>
       <c r="T187" s="5"/>
@@ -34148,7 +35691,7 @@
       <c r="AF187" s="5"/>
       <c r="AG187" s="5"/>
     </row>
-    <row r="188" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A188" s="11">
         <v>0</v>
       </c>
@@ -34164,20 +35707,54 @@
         <f>SLOPE(B178:Q178,$B$161:$Q$161)</f>
         <v>0</v>
       </c>
-      <c r="E188" s="7"/>
-      <c r="F188" s="7"/>
-      <c r="G188" s="7"/>
-      <c r="I188" s="7"/>
-      <c r="J188" s="7"/>
-      <c r="K188" s="7"/>
-      <c r="L188" s="7"/>
-      <c r="M188" s="7"/>
-      <c r="N188" s="7"/>
-      <c r="O188" s="7"/>
-      <c r="P188" s="7"/>
+      <c r="E188" s="11">
+        <v>0</v>
+      </c>
+      <c r="F188" s="18" t="e">
+        <f>$E188/B188</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G188" s="18" t="e">
+        <f t="shared" ref="G188:H188" si="163">$E188/C188</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H188" s="18" t="e">
+        <f t="shared" si="163"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I188" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="J188" s="20">
+        <f>(SLOPE(F189:F195,$E$189:$E$195)^(-1))</f>
+        <v>1.8854738728565234E-4</v>
+      </c>
+      <c r="K188" s="20">
+        <f t="shared" ref="K188:L188" si="164">(SLOPE(G189:G195,$E$189:$E$195)^(-1))</f>
+        <v>4.7846728576838497E-5</v>
+      </c>
+      <c r="L188" s="20">
+        <f t="shared" si="164"/>
+        <v>4.4760299419995727E-5</v>
+      </c>
+      <c r="M188" s="11">
+        <v>0</v>
+      </c>
+      <c r="N188" s="17" t="e">
+        <f>(N$187)/(($J$188*$M188)/($B188*($J$189+$M188))-1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O188" s="17" t="e">
+        <f t="shared" ref="O188:P188" si="165">(O$187)/(($J$188*$M188)/($B188*($J$189+$M188))-1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P188" s="17" t="e">
+        <f t="shared" si="165"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="Q188" s="7"/>
     </row>
-    <row r="189" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A189" s="11">
         <v>0.25</v>
       </c>
@@ -34186,172 +35763,321 @@
         <v>8.2310961232144069E-5</v>
       </c>
       <c r="C189" s="7">
-        <f t="shared" ref="C189:C195" si="163">SLOPE(B171:Q171,$B$161:$Q$161)</f>
+        <f t="shared" ref="C189:C195" si="166">SLOPE(B171:Q171,$B$161:$Q$161)</f>
         <v>7.6424826954288411E-5</v>
       </c>
       <c r="D189" s="7">
-        <f t="shared" ref="D189:D195" si="164">SLOPE(B179:Q179,$B$161:$Q$161)</f>
+        <f t="shared" ref="D189:D195" si="167">SLOPE(B179:Q179,$B$161:$Q$161)</f>
         <v>3.7706127734992981E-5</v>
       </c>
-      <c r="E189" s="7"/>
-      <c r="F189" s="7"/>
-      <c r="G189" s="7"/>
-      <c r="I189" s="7"/>
-      <c r="J189" s="7"/>
-      <c r="K189" s="7"/>
-      <c r="L189" s="7"/>
-      <c r="M189" s="7"/>
-      <c r="N189" s="7"/>
-      <c r="O189" s="7"/>
-      <c r="P189" s="7"/>
+      <c r="E189" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="F189" s="18">
+        <f t="shared" ref="F189:F195" si="168">$E189/B189</f>
+        <v>3037.2625499405544</v>
+      </c>
+      <c r="G189" s="18">
+        <f>$E189/C189</f>
+        <v>3271.1883031090306</v>
+      </c>
+      <c r="H189" s="18">
+        <f t="shared" ref="H189:H195" si="169">$E189/D189</f>
+        <v>6630.2220625001692</v>
+      </c>
+      <c r="I189" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="J189" s="20">
+        <f>INTERCEPT(F189:F195,$E$189:$E$195)*J188</f>
+        <v>6.0668872573680033E-2</v>
+      </c>
+      <c r="K189" s="20">
+        <f t="shared" ref="K189:L189" si="170">INTERCEPT(G189:G195,$E$189:$E$195)*K188</f>
+        <v>-0.62519372057743106</v>
+      </c>
+      <c r="L189" s="20">
+        <f t="shared" si="170"/>
+        <v>-0.25332872556303637</v>
+      </c>
+      <c r="M189" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="N189" s="17">
+        <f t="shared" ref="N189:P195" si="171">(N$187)/(($J$188*$M189)/($B189*($J$189+$M189))-1)</f>
+        <v>0</v>
+      </c>
+      <c r="O189" s="17">
+        <f t="shared" si="171"/>
+        <v>7.1145802471631328</v>
+      </c>
+      <c r="P189" s="17">
+        <f t="shared" si="171"/>
+        <v>14.229160494326266</v>
+      </c>
       <c r="Q189" s="7"/>
     </row>
-    <row r="190" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A190" s="11">
         <v>0.5</v>
       </c>
       <c r="B190" s="7">
-        <f t="shared" ref="B190:B194" si="165">SLOPE(B164:Q164,$B$161:$Q$161)</f>
+        <f t="shared" ref="B190:B194" si="172">SLOPE(B164:Q164,$B$161:$Q$161)</f>
         <v>1.3877202506865807E-4</v>
       </c>
       <c r="C190" s="7">
-        <f t="shared" si="163"/>
+        <f t="shared" si="166"/>
         <v>1.0332114762069779E-4</v>
       </c>
       <c r="D190" s="7">
-        <f t="shared" si="164"/>
+        <f t="shared" si="167"/>
         <v>3.638429772751105E-5</v>
       </c>
-      <c r="E190" s="7"/>
-      <c r="F190" s="7"/>
-      <c r="G190" s="7"/>
+      <c r="E190" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F190" s="18">
+        <f t="shared" si="168"/>
+        <v>3603.0316611191834</v>
+      </c>
+      <c r="G190" s="18">
+        <f t="shared" ref="G189:G195" si="173">$E190/C190</f>
+        <v>4839.2803556107383</v>
+      </c>
+      <c r="H190" s="18">
+        <f t="shared" si="169"/>
+        <v>13742.191858273463</v>
+      </c>
       <c r="I190" s="7"/>
       <c r="J190" s="7"/>
       <c r="K190" s="7"/>
       <c r="L190" s="7"/>
-      <c r="M190" s="7"/>
-      <c r="N190" s="7"/>
-      <c r="O190" s="7"/>
-      <c r="P190" s="7"/>
+      <c r="M190" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="N190" s="17">
+        <f t="shared" si="171"/>
+        <v>0</v>
+      </c>
+      <c r="O190" s="17">
+        <f t="shared" si="171"/>
+        <v>28.346833597663434</v>
+      </c>
+      <c r="P190" s="17">
+        <f t="shared" si="171"/>
+        <v>56.693667195326867</v>
+      </c>
       <c r="Q190" s="7"/>
     </row>
-    <row r="191" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A191" s="11">
         <v>1</v>
       </c>
       <c r="B191" s="7">
-        <f t="shared" si="165"/>
+        <f t="shared" si="172"/>
         <v>2.1929899430917334E-4</v>
       </c>
       <c r="C191" s="7">
-        <f t="shared" si="163"/>
+        <f t="shared" si="166"/>
         <v>1.1144662467556151E-4</v>
       </c>
       <c r="D191" s="7">
-        <f t="shared" si="164"/>
+        <f t="shared" si="167"/>
         <v>6.1773974200472767E-5</v>
       </c>
-      <c r="E191" s="7"/>
-      <c r="F191" s="7"/>
-      <c r="G191" s="7"/>
+      <c r="E191" s="11">
+        <v>1</v>
+      </c>
+      <c r="F191" s="18">
+        <f>$E191/B191</f>
+        <v>4559.984431985923</v>
+      </c>
+      <c r="G191" s="18">
+        <f t="shared" si="173"/>
+        <v>8972.9052172836618</v>
+      </c>
+      <c r="H191" s="18">
+        <f t="shared" si="169"/>
+        <v>16188.047036681457</v>
+      </c>
       <c r="I191" s="7"/>
       <c r="J191" s="7"/>
       <c r="K191" s="7"/>
       <c r="L191" s="7"/>
-      <c r="M191" s="7"/>
-      <c r="N191" s="7"/>
-      <c r="O191" s="7"/>
-      <c r="P191" s="7"/>
+      <c r="M191" s="11">
+        <v>1</v>
+      </c>
+      <c r="N191" s="17">
+        <f t="shared" si="171"/>
+        <v>0</v>
+      </c>
+      <c r="O191" s="17">
+        <f t="shared" si="171"/>
+        <v>-31.678191932296826</v>
+      </c>
+      <c r="P191" s="17">
+        <f t="shared" si="171"/>
+        <v>-63.356383864593653</v>
+      </c>
       <c r="Q191" s="7"/>
     </row>
-    <row r="192" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A192" s="11">
         <v>2</v>
       </c>
       <c r="B192" s="7">
-        <f t="shared" si="165"/>
+        <f t="shared" si="172"/>
         <v>2.0796976571816188E-4</v>
       </c>
       <c r="C192" s="7">
-        <f t="shared" si="163"/>
+        <f t="shared" si="166"/>
         <v>6.8901702432589684E-5</v>
       </c>
       <c r="D192" s="7">
-        <f t="shared" si="164"/>
+        <f t="shared" si="167"/>
         <v>6.1066202904346619E-5</v>
       </c>
-      <c r="E192" s="7"/>
-      <c r="F192" s="7"/>
-      <c r="G192" s="7"/>
+      <c r="E192" s="11">
+        <v>2</v>
+      </c>
+      <c r="F192" s="18">
+        <f t="shared" si="168"/>
+        <v>9616.7824832306433</v>
+      </c>
+      <c r="G192" s="18">
+        <f t="shared" si="173"/>
+        <v>29026.858980105895</v>
+      </c>
+      <c r="H192" s="18">
+        <f t="shared" si="169"/>
+        <v>32751.340428563675</v>
+      </c>
       <c r="I192" s="7"/>
       <c r="J192" s="7"/>
       <c r="K192" s="7"/>
       <c r="L192" s="7"/>
-      <c r="M192" s="7"/>
-      <c r="N192" s="7"/>
-      <c r="O192" s="7"/>
-      <c r="P192" s="7"/>
+      <c r="M192" s="11">
+        <v>2</v>
+      </c>
+      <c r="N192" s="17">
+        <f t="shared" si="171"/>
+        <v>0</v>
+      </c>
+      <c r="O192" s="17">
+        <f>(O$187)/(($J$188*$M192)/($B192*($J$189+$M192))-1)</f>
+        <v>-49.965771511586212</v>
+      </c>
+      <c r="P192" s="17">
+        <f t="shared" si="171"/>
+        <v>-99.931543023172424</v>
+      </c>
       <c r="Q192" s="7"/>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A193" s="11">
         <v>5</v>
       </c>
       <c r="B193" s="7">
-        <f t="shared" si="165"/>
+        <f t="shared" si="172"/>
         <v>1.9650144609349769E-4</v>
       </c>
       <c r="C193" s="7">
-        <f t="shared" si="163"/>
+        <f t="shared" si="166"/>
         <v>7.0465433323288246E-5</v>
       </c>
       <c r="D193" s="7">
-        <f t="shared" si="164"/>
+        <f t="shared" si="167"/>
         <v>5.5308553072597458E-5</v>
       </c>
-      <c r="E193" s="7"/>
-      <c r="F193" s="7"/>
-      <c r="G193" s="7"/>
+      <c r="E193" s="11">
+        <v>5</v>
+      </c>
+      <c r="F193" s="18">
+        <f t="shared" si="168"/>
+        <v>25445.105363860486</v>
+      </c>
+      <c r="G193" s="18">
+        <f t="shared" si="173"/>
+        <v>70956.776453222221</v>
+      </c>
+      <c r="H193" s="18">
+        <f t="shared" si="169"/>
+        <v>90401.931025695958</v>
+      </c>
       <c r="I193" s="7"/>
       <c r="J193" s="7"/>
       <c r="K193" s="7"/>
       <c r="L193" s="7"/>
-      <c r="M193" s="7"/>
-      <c r="N193" s="7"/>
-      <c r="O193" s="7"/>
-      <c r="P193" s="7"/>
+      <c r="M193" s="11">
+        <v>5</v>
+      </c>
+      <c r="N193" s="17">
+        <f t="shared" si="171"/>
+        <v>0</v>
+      </c>
+      <c r="O193" s="17">
+        <f t="shared" si="171"/>
+        <v>-115.42586545071727</v>
+      </c>
+      <c r="P193" s="17">
+        <f t="shared" si="171"/>
+        <v>-230.85173090143454</v>
+      </c>
       <c r="Q193" s="7"/>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A194" s="11">
         <v>7</v>
       </c>
       <c r="B194" s="7">
-        <f t="shared" si="165"/>
+        <f t="shared" si="172"/>
         <v>1.7517501290123882E-4</v>
       </c>
       <c r="C194" s="7">
-        <f t="shared" si="163"/>
+        <f t="shared" si="166"/>
         <v>6.7675269156013007E-5</v>
       </c>
       <c r="D194" s="7">
-        <f t="shared" si="164"/>
+        <f t="shared" si="167"/>
         <v>4.7569883214723198E-5</v>
       </c>
-      <c r="E194" s="7"/>
-      <c r="F194" s="7"/>
-      <c r="G194" s="7"/>
+      <c r="E194" s="11">
+        <v>7</v>
+      </c>
+      <c r="F194" s="18">
+        <f t="shared" si="168"/>
+        <v>39960.037017074465</v>
+      </c>
+      <c r="G194" s="18">
+        <f t="shared" si="173"/>
+        <v>103435.12611472257</v>
+      </c>
+      <c r="H194" s="18">
+        <f t="shared" si="169"/>
+        <v>147151.92737394513</v>
+      </c>
       <c r="I194" s="7"/>
       <c r="J194" s="7"/>
       <c r="K194" s="7"/>
       <c r="L194" s="7"/>
-      <c r="M194" s="7"/>
-      <c r="N194" s="7"/>
-      <c r="O194" s="7"/>
-      <c r="P194" s="7"/>
+      <c r="M194" s="11">
+        <v>7</v>
+      </c>
+      <c r="N194" s="17">
+        <f t="shared" si="171"/>
+        <v>0</v>
+      </c>
+      <c r="O194" s="17">
+        <f t="shared" si="171"/>
+        <v>89.433724471037124</v>
+      </c>
+      <c r="P194" s="17">
+        <f t="shared" si="171"/>
+        <v>178.86744894207425</v>
+      </c>
       <c r="Q194" s="7"/>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A195" s="11">
         <v>10</v>
       </c>
@@ -34360,27 +36086,50 @@
         <v>1.9011179997378887E-4</v>
       </c>
       <c r="C195" s="7">
-        <f t="shared" si="163"/>
+        <f t="shared" si="166"/>
         <v>4.4206997873103683E-5</v>
       </c>
       <c r="D195" s="7">
-        <f t="shared" si="164"/>
+        <f t="shared" si="167"/>
         <v>4.3705680871439547E-5</v>
       </c>
-      <c r="E195" s="7"/>
-      <c r="F195" s="7"/>
-      <c r="G195" s="7"/>
+      <c r="E195" s="11">
+        <v>10</v>
+      </c>
+      <c r="F195" s="18">
+        <f t="shared" si="168"/>
+        <v>52600.627637941056</v>
+      </c>
+      <c r="G195" s="18">
+        <f t="shared" si="173"/>
+        <v>226208.52989621754</v>
+      </c>
+      <c r="H195" s="18">
+        <f t="shared" si="169"/>
+        <v>228803.20820112707</v>
+      </c>
       <c r="I195" s="7"/>
       <c r="J195" s="7"/>
       <c r="K195" s="7"/>
       <c r="L195" s="7"/>
-      <c r="M195" s="7"/>
-      <c r="N195" s="7"/>
-      <c r="O195" s="7"/>
-      <c r="P195" s="7"/>
+      <c r="M195" s="11">
+        <v>10</v>
+      </c>
+      <c r="N195" s="17">
+        <f>(N$187)/(($J$188*$M195)/($B195*($J$189+$M195))-1)</f>
+        <v>0</v>
+      </c>
+      <c r="O195" s="17">
+        <f t="shared" si="171"/>
+        <v>-422.25009682855728</v>
+      </c>
+      <c r="P195" s="17">
+        <f t="shared" si="171"/>
+        <v>-844.50019365711455</v>
+      </c>
       <c r="Q195" s="7"/>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A196" s="11"/>
       <c r="B196" s="7"/>
       <c r="C196" s="7"/>
@@ -34399,7 +36148,7 @@
       <c r="P196" s="7"/>
       <c r="Q196" s="7"/>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A197" s="10"/>
       <c r="B197" s="7"/>
       <c r="C197" s="7"/>
@@ -34418,7 +36167,7 @@
       <c r="P197" s="7"/>
       <c r="Q197" s="7"/>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A198" s="10"/>
       <c r="B198" s="7"/>
       <c r="C198" s="7"/>
@@ -34437,7 +36186,7 @@
       <c r="P198" s="7"/>
       <c r="Q198" s="7"/>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A199" s="10"/>
       <c r="B199" s="7"/>
       <c r="C199" s="7"/>
@@ -34456,7 +36205,7 @@
       <c r="P199" s="7"/>
       <c r="Q199" s="7"/>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A200" s="10"/>
       <c r="B200" s="7"/>
       <c r="C200" s="7"/>
@@ -34475,7 +36224,7 @@
       <c r="P200" s="7"/>
       <c r="Q200" s="7"/>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A201" s="10"/>
       <c r="B201" s="7"/>
       <c r="C201" s="7"/>
@@ -34494,7 +36243,7 @@
       <c r="P201" s="7"/>
       <c r="Q201" s="7"/>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A202" s="10"/>
       <c r="B202" s="7"/>
       <c r="C202" s="7"/>
@@ -34513,7 +36262,7 @@
       <c r="P202" s="7"/>
       <c r="Q202" s="7"/>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A203" s="10"/>
       <c r="B203" s="7"/>
       <c r="C203" s="7"/>
@@ -34532,7 +36281,7 @@
       <c r="P203" s="7"/>
       <c r="Q203" s="7"/>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A204" s="9"/>
       <c r="B204" s="7"/>
       <c r="C204" s="7"/>
@@ -34551,7 +36300,7 @@
       <c r="P204" s="7"/>
       <c r="Q204" s="7"/>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A205" s="9"/>
       <c r="B205" s="7"/>
       <c r="C205" s="7"/>
@@ -34570,7 +36319,7 @@
       <c r="P205" s="7"/>
       <c r="Q205" s="7"/>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A206" s="9"/>
       <c r="B206" s="7"/>
       <c r="C206" s="7"/>
@@ -34589,7 +36338,7 @@
       <c r="P206" s="7"/>
       <c r="Q206" s="7"/>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A207" s="9"/>
       <c r="B207" s="7"/>
       <c r="C207" s="7"/>
@@ -34608,7 +36357,7 @@
       <c r="P207" s="7"/>
       <c r="Q207" s="7"/>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A208" s="9"/>
       <c r="B208" s="7"/>
       <c r="C208" s="7"/>
@@ -34627,7 +36376,7 @@
       <c r="P208" s="7"/>
       <c r="Q208" s="7"/>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A209" s="9"/>
       <c r="B209" s="7"/>
       <c r="C209" s="7"/>
@@ -34646,7 +36395,7 @@
       <c r="P209" s="7"/>
       <c r="Q209" s="7"/>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A210" s="9"/>
       <c r="B210" s="7"/>
       <c r="C210" s="7"/>
@@ -34665,7 +36414,7 @@
       <c r="P210" s="7"/>
       <c r="Q210" s="7"/>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A211" s="9"/>
       <c r="B211" s="7"/>
       <c r="C211" s="7"/>
@@ -34685,18 +36434,19 @@
       <c r="Q211" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B160:Q160"/>
-    <mergeCell ref="R160:AG160"/>
-    <mergeCell ref="R186:AG186"/>
-    <mergeCell ref="A186:D186"/>
-    <mergeCell ref="E186:G186"/>
+  <mergeCells count="12">
     <mergeCell ref="B32:Q32"/>
     <mergeCell ref="S32:AH32"/>
     <mergeCell ref="B107:Q107"/>
     <mergeCell ref="R107:AG107"/>
     <mergeCell ref="B134:Q134"/>
     <mergeCell ref="R134:AG134"/>
+    <mergeCell ref="B160:Q160"/>
+    <mergeCell ref="R160:AG160"/>
+    <mergeCell ref="R186:AG186"/>
+    <mergeCell ref="A186:D186"/>
+    <mergeCell ref="E186:H186"/>
+    <mergeCell ref="N186:P186"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -34711,7 +36461,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>